<commit_message>
ControlDbp begin rationalizing commands
</commit_message>
<xml_diff>
--- a/docs/DBPA manager web service URIs.xlsx
+++ b/docs/DBPA manager web service URIs.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ron\Documents\My Projects\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commands!$B$1:$B$34</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -271,7 +266,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -626,7 +621,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -641,16 +636,16 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="48.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
@@ -664,7 +659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -679,7 +674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
@@ -694,7 +689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -709,7 +704,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -724,7 +719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -739,7 +734,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,7 +749,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -769,7 +764,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -784,7 +779,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -799,7 +794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -814,7 +809,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -829,7 +824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -844,7 +839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -859,7 +854,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -874,7 +869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -889,7 +884,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -904,7 +899,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -919,7 +914,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -934,7 +929,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -949,7 +944,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -964,7 +959,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
@@ -979,7 +974,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -994,7 +989,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1009,7 +1004,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
@@ -1024,37 +1019,37 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SHOW</v>
+        <f>LEFT(A26,SEARCH(" ",A26)-1)</f>
+        <v>STOP</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>STOP</v>
+        <v>SHOW</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -1069,7 +1064,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1084,7 +1079,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1099,7 +1094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1114,7 +1109,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -1129,7 +1124,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -1144,7 +1139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
@@ -1175,9 +1170,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="102.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ControlDbp near complete rationalized command set
</commit_message>
<xml_diff>
--- a/docs/DBPA manager web service URIs.xlsx
+++ b/docs/DBPA manager web service URIs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\hauldata\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12216"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commands!$B$1:$B$34</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -163,9 +168,6 @@
     <t>LIST SCHEDULES [LIKE 'likeName']</t>
   </si>
   <si>
-    <t>SHOW SCHEDULES [LIKE 'likeName']</t>
-  </si>
-  <si>
     <t>LIST SCRIPTS [LIKE 'likeName']</t>
   </si>
   <si>
@@ -262,11 +264,14 @@
   <si>
     <t>SHOW SCRIPT scriptName</t>
   </si>
+  <si>
+    <t>-- not implemented --</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -304,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -315,6 +320,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,7 +629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -636,21 +644,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="1"/>
-    <col min="4" max="4" width="48.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="54.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>8</v>
@@ -659,7 +667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -674,9 +682,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" ref="B3" si="0">LEFT(A3,SEARCH(" ",A3)-1)</f>
@@ -689,7 +697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -704,7 +712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -719,22 +727,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,7 +757,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -764,7 +772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -779,7 +787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -794,7 +802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -806,10 +814,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -824,7 +832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -839,22 +847,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>SHOW</v>
+        <v>LIST</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -869,22 +877,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>45</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>LIST</v>
+        <v>--</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -899,9 +907,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -914,9 +922,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -929,7 +937,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -944,7 +952,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -959,22 +967,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1" t="str">
         <f t="shared" si="1"/>
         <v>UPDATE</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -989,7 +997,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1004,9 +1012,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1019,9 +1027,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1" t="str">
         <f>LEFT(A26,SEARCH(" ",A26)-1)</f>
@@ -1034,9 +1042,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1049,9 +1057,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1064,7 +1072,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1079,7 +1087,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1094,7 +1102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1109,7 +1117,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -1124,7 +1132,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -1139,7 +1147,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
@@ -1170,17 +1178,17 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1196,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1196,23 +1204,23 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1220,7 +1228,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ControlDbp implements PUT and GET SCRIPT
</commit_message>
<xml_diff>
--- a/docs/DBPA manager web service URIs.xlsx
+++ b/docs/DBPA manager web service URIs.xlsx
@@ -114,18 +114,6 @@
     <t>STOP MANAGER</t>
   </si>
   <si>
-    <t>PUT SCRIPT scriptName FROM scriptDir</t>
-  </si>
-  <si>
-    <t>GET SCRIPT scriptName TO scriptDir</t>
-  </si>
-  <si>
-    <t>PUT PROPERTIES propName FROM propDir</t>
-  </si>
-  <si>
-    <t>GET PROPERTIES propName TO propDir</t>
-  </si>
-  <si>
     <t>VALIDATE SCHEDULE schedName</t>
   </si>
   <si>
@@ -266,6 +254,18 @@
   </si>
   <si>
     <t>-- not implemented --</t>
+  </si>
+  <si>
+    <t>PUT SCRIPT scriptName</t>
+  </si>
+  <si>
+    <t>GET SCRIPT scriptName</t>
+  </si>
+  <si>
+    <t>PUT PROPERTIES propName</t>
+  </si>
+  <si>
+    <t>GET PROPERTIES propName</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>8</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>LEFT(A2,SEARCH(" ",A2)-1)</f>
@@ -684,7 +684,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" ref="B3" si="0">LEFT(A3,SEARCH(" ",A3)-1)</f>
@@ -699,7 +699,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" ref="B4:B34" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
@@ -729,7 +729,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="1"/>
@@ -739,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -754,12 +754,12 @@
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="1"/>
@@ -774,7 +774,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -804,22 +804,22 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="1"/>
@@ -849,7 +849,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="1"/>
@@ -859,7 +859,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,7 +879,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -889,12 +889,12 @@
         <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="1"/>
@@ -904,12 +904,12 @@
         <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -919,12 +919,12 @@
         <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -969,22 +969,22 @@
     </row>
     <row r="22" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1" t="str">
         <f t="shared" si="1"/>
         <v>UPDATE</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="str">
         <f t="shared" si="1"/>
@@ -994,12 +994,12 @@
         <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1009,12 +1009,12 @@
         <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1024,12 +1024,12 @@
         <v>13</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="str">
         <f>LEFT(A26,SEARCH(" ",A26)-1)</f>
@@ -1039,12 +1039,12 @@
         <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1054,12 +1054,12 @@
         <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1069,7 +1069,7 @@
         <v>10</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1185,10 +1185,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,23 +1204,23 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
         <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
         <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1228,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised semantics of properties resource; Removed propName attribute of Job; Respect ControlDbp.path.properties and ManageDbp.path.properties; Store schedules as .sch files local to ControlDbp; Refactor dbpa-control web clients to use FilesResource
</commit_message>
<xml_diff>
--- a/docs/DBPA manager web service URIs.xlsx
+++ b/docs/DBPA manager web service URIs.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\hauldata\docs\"/>
@@ -186,16 +186,66 @@
     <t>STOP JOB runId</t>
   </si>
   <si>
+    <t>schedules/[?like={likeName}]</t>
+  </si>
+  <si>
+    <t>Silently retrieve an object from remote to local</t>
+  </si>
+  <si>
+    <t>SHOW</t>
+  </si>
+  <si>
+    <t>LIST</t>
+  </si>
+  <si>
+    <t>Delete a single object</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Display the content of a single object by name or ID</t>
+  </si>
+  <si>
+    <t>Display multiple objects in single-line format; if objects naturally span multiple lines, only display object names</t>
+  </si>
+  <si>
+    <t>Store a single object</t>
+  </si>
+  <si>
+    <t>SHOW SCRIPT scriptName</t>
+  </si>
+  <si>
+    <t>-- not implemented --</t>
+  </si>
+  <si>
+    <t>PUT SCRIPT scriptName</t>
+  </si>
+  <si>
+    <t>GET SCRIPT scriptName</t>
+  </si>
+  <si>
+    <t>PUT PROPERTIES propName</t>
+  </si>
+  <si>
+    <t>GET PROPERTIES propName</t>
+  </si>
+  <si>
     <t>PUT JOB jobName SCRIPT scriptName
-[NO PROPERTIES | PROPERTIES propName]
 [NO ARGUMENTS | ARGUMENTS argName1 argValue1 [, …]]
 [NO SCHEDULE[S] | SCHEDULE[S] schedName1 [, …]]
 [ENABLED {ON | OFF}]</t>
   </si>
   <si>
+    <t>UPDATE JOB jobName [SCRIPT scriptName]
+[NO ARGUMENTS |
+ARGUMENTS argName1 argValue1 [, …]]
+[NO SCHEDULE[S] |
+SCHEDULE[S] schedName1 [, …]]
+[ENABLED {ON | OFF}]</t>
+  </si>
+  <si>
     <t>jobs/{jobName}/script
-jobs/{jobName}/propfile
-jobs/{jobName}/propfile
 jobs/{jobName}/arguments
 jobs/{jobName}/arguments
 jobs/{jobName}/schedules
@@ -208,64 +258,7 @@
 PUT
 DELETE
 PUT
-DELETE
-PUT
 PUT</t>
-  </si>
-  <si>
-    <t>UPDATE JOB jobName [SCRIPT scriptName]
-[NO PROPERTIES |
-PROPERTIES propName]
-[NO ARGUMENTS |
-ARGUMENTS argName1 argValue1 [, …]]
-[NO SCHEDULE[S] |
-SCHEDULE[S] schedName1 [, …]]
-[ENABLED {ON | OFF}]</t>
-  </si>
-  <si>
-    <t>schedules/[?like={likeName}]</t>
-  </si>
-  <si>
-    <t>Silently retrieve an object from remote to local</t>
-  </si>
-  <si>
-    <t>SHOW</t>
-  </si>
-  <si>
-    <t>LIST</t>
-  </si>
-  <si>
-    <t>Delete a single object</t>
-  </si>
-  <si>
-    <t>Usage</t>
-  </si>
-  <si>
-    <t>Display the content of a single object by name or ID</t>
-  </si>
-  <si>
-    <t>Display multiple objects in single-line format; if objects naturally span multiple lines, only display object names</t>
-  </si>
-  <si>
-    <t>Store a single object</t>
-  </si>
-  <si>
-    <t>SHOW SCRIPT scriptName</t>
-  </si>
-  <si>
-    <t>-- not implemented --</t>
-  </si>
-  <si>
-    <t>PUT SCRIPT scriptName</t>
-  </si>
-  <si>
-    <t>GET SCRIPT scriptName</t>
-  </si>
-  <si>
-    <t>PUT PROPERTIES propName</t>
-  </si>
-  <si>
-    <t>GET PROPERTIES propName</t>
   </si>
 </sst>
 </file>
@@ -641,7 +634,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +662,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>LEFT(A2,SEARCH(" ",A2)-1)</f>
@@ -684,7 +677,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" ref="B3" si="0">LEFT(A3,SEARCH(" ",A3)-1)</f>
@@ -699,7 +692,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" ref="B4:B34" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
@@ -759,7 +752,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="1"/>
@@ -774,7 +767,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -859,7 +852,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,7 +872,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -922,9 +915,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -967,19 +960,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="str">
         <f t="shared" si="1"/>
         <v>UPDATE</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,7 +1181,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1196,7 +1189,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,23 +1197,23 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
         <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1221,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement START JOB argument replacement
</commit_message>
<xml_diff>
--- a/docs/DBPA manager web service URIs.xlsx
+++ b/docs/DBPA manager web service URIs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>Verb</t>
   </si>
   <si>
-    <t>START JOB jobName</t>
-  </si>
-  <si>
     <t>STOP JOB runId</t>
   </si>
   <si>
@@ -260,11 +257,14 @@
 PUT
 PUT</t>
   </si>
+  <si>
+    <t>START JOB jobName [ARGUMENTS argName1 argValue1 [, …]]]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -629,17 +629,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -662,7 +662,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>LEFT(A2,SEARCH(" ",A2)-1)</f>
@@ -677,7 +677,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" ref="B3" si="0">LEFT(A3,SEARCH(" ",A3)-1)</f>
@@ -692,7 +692,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" ref="B4:B34" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
@@ -752,7 +752,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="1"/>
@@ -767,7 +767,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -852,7 +852,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -872,7 +872,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -917,7 +917,7 @@
     </row>
     <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -962,17 +962,17 @@
     </row>
     <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1007,7 +1007,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="str">
         <f>LEFT(A26,SEARCH(" ",A26)-1)</f>
@@ -1156,14 +1156,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B34"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1181,7 +1180,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1189,7 +1188,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1197,23 +1196,23 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1221,7 +1220,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ControlDbp: added CREATE SCHEDULE command; renamed PUT JOB to CREATE JOB
</commit_message>
<xml_diff>
--- a/docs/DBPA manager web service URIs.xlsx
+++ b/docs/DBPA manager web service URIs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,7 +16,7 @@
     <sheet name="Usage" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commands!$B$1:$B$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commands!$B$1:$B$35</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
   <si>
     <t>VALIDATE SCRIPT scriptName</t>
   </si>
@@ -117,9 +117,6 @@
     <t>VALIDATE SCHEDULE schedName</t>
   </si>
   <si>
-    <t>PUT SCHEDULE schedName ‘schedule’</t>
-  </si>
-  <si>
     <t>scripts/-/validations/{scriptName}</t>
   </si>
   <si>
@@ -226,12 +223,6 @@
   </si>
   <si>
     <t>GET PROPERTIES propName</t>
-  </si>
-  <si>
-    <t>PUT JOB jobName SCRIPT scriptName
-[NO ARGUMENTS | ARGUMENTS argName1 argValue1 [, …]]
-[NO SCHEDULE[S] | SCHEDULE[S] schedName1 [, …]]
-[ENABLED {ON | OFF}]</t>
   </si>
   <si>
     <t>UPDATE JOB jobName [SCRIPT scriptName]
@@ -260,12 +251,24 @@
   <si>
     <t>START JOB jobName [ARGUMENTS argName1 argValue1 [, …]]]</t>
   </si>
+  <si>
+    <t>CREATE SCHEDULE schedName ‘schedule’</t>
+  </si>
+  <si>
+    <t>CREATE JOB jobName SCRIPT scriptName
+[NO ARGUMENTS | ARGUMENTS argName1 argValue1 [, …]]
+[NO SCHEDULE[S] | SCHEDULE[S] schedName1 [, …]]
+[ENABLED {ON | OFF}]</t>
+  </si>
+  <si>
+    <t>PUT SCHEDULE schedName</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +278,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -304,17 +322,17 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,7 +648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -639,19 +657,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="57" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="4"/>
+    <col min="4" max="4" width="48.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>8</v>
@@ -661,497 +679,512 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="1" t="str">
+      <c r="A2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="4" t="str">
         <f>LEFT(A2,SEARCH(" ",A2)-1)</f>
         <v>PUT</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="1" t="str">
+      <c r="A3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="4" t="str">
         <f t="shared" ref="B3" si="0">LEFT(A3,SEARCH(" ",A3)-1)</f>
         <v>SHOW</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <f t="shared" ref="B4:B35" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
+        <v>GET</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>VALIDATE</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="1" t="str">
-        <f t="shared" ref="B4:B34" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
+      <c r="B8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="4" t="str">
+        <f t="shared" si="1"/>
         <v>GET</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="str">
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>DELETE</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="1" t="str">
+      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>LIST</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="str">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="4" t="str">
+        <f t="shared" ref="B12" si="2">LEFT(A12,SEARCH(" ",A12)-1)</f>
+        <v>CREATE</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>SHOW</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>--</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>VALIDATE</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-      <c r="C8" s="1" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CREATE</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="D20" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>SHOW</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>GET</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B23" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>START</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="4" t="str">
+        <f>LEFT(A27,SEARCH(" ",A27)-1)</f>
+        <v>STOP</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="1" t="str">
+      <c r="D27" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>SHOW</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="4" t="str">
         <f t="shared" si="1"/>
         <v>LIST</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="C29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>STOP</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>START</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SHOW</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D31" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CONFIRM</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>STOP</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>--</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>VALIDATE</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D33" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CREATE</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SHOW</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>START</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="1" t="str">
-        <f>LEFT(A26,SEARCH(" ",A26)-1)</f>
-        <v>STOP</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SHOW</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>STOP</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>START</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="1" t="str">
+      <c r="D34" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="4" t="str">
         <f t="shared" si="1"/>
         <v>CONFIRM</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>STOP</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CREATE</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CONFIRM</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="C35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1175,12 +1208,12 @@
     <col min="2" max="2" width="102.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>56</v>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1221,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1196,23 +1229,23 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1220,7 +1253,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented ControlDbp UPDATE SCHEDULE; assure schedules stop when a job is updated if appropriate
</commit_message>
<xml_diff>
--- a/docs/DBPA manager web service URIs.xlsx
+++ b/docs/DBPA manager web service URIs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,7 +16,7 @@
     <sheet name="Usage" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commands!$B$1:$B$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commands!$B$1:$B$36</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="74">
   <si>
     <t>VALIDATE SCRIPT scriptName</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>PUT SCHEDULE schedName</t>
+  </si>
+  <si>
+    <t>UPDATE SCHEDULE schedName ‘schedule’</t>
+  </si>
+  <si>
+    <t>schedules/{schedName}/body</t>
   </si>
 </sst>
 </file>
@@ -320,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -333,6 +339,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,7 +657,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -713,7 +722,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="4" t="str">
-        <f t="shared" ref="B4:B35" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
+        <f t="shared" ref="B4:B36" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
         <v>GET</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -844,30 +853,30 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>71</v>
+      <c r="A13" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="B13" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
+        <f t="shared" ref="B13" si="3">LEFT(A13,SEARCH(" ",A13)-1)</f>
+        <v>UPDATE</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>18</v>
+      <c r="D13" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>SHOW</v>
+        <v>PUT</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>18</v>
@@ -875,104 +884,104 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>LIST</v>
+        <v>SHOW</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="str">
+      <c r="B17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>DELETE</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="4" t="str">
+      <c r="B18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>--</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>VALIDATE</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>VALIDATE</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="4" t="str">
+      <c r="B20" s="4" t="str">
         <f t="shared" si="1"/>
         <v>LIST</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="4" t="str">
+      <c r="B21" s="4" t="str">
         <f t="shared" si="1"/>
         <v>CREATE</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>SHOW</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>19</v>
@@ -980,52 +989,52 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v>SHOW</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="4" t="str">
+      <c r="B24" s="4" t="str">
         <f t="shared" si="1"/>
         <v>UPDATE</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1035,49 +1044,49 @@
         <v>10</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="B26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>START</v>
+        <v>LIST</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B27" s="4" t="str">
-        <f>LEFT(A27,SEARCH(" ",A27)-1)</f>
-        <v>STOP</v>
+        <f t="shared" si="1"/>
+        <v>START</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B28" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>SHOW</v>
+        <f>LEFT(A28,SEARCH(" ",A28)-1)</f>
+        <v>STOP</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>33</v>
@@ -1085,44 +1094,44 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>LIST</v>
+        <v>SHOW</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>STOP</v>
+        <v>LIST</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B31" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>START</v>
+        <v>STOP</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>22</v>
@@ -1130,14 +1139,14 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>CONFIRM</v>
+        <v>START</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>22</v>
@@ -1145,46 +1154,61 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B33" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>STOP</v>
+        <v>CONFIRM</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B34" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>CREATE</v>
+        <v>STOP</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CREATE</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="4" t="str">
+      <c r="B36" s="4" t="str">
         <f t="shared" si="1"/>
         <v>CONFIRM</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="4" t="s">
+      <c r="C36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ManageDbp ability to run a script directly without a job
</commit_message>
<xml_diff>
--- a/docs/DBPA manager web service URIs.xlsx
+++ b/docs/DBPA manager web service URIs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\hauldata\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A947BAD3-47CE-4CF9-984C-75534FDF28CC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593F0DCD-3063-4D9F-ABD8-C5F806C9CEAC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,9 @@
     <sheet name="Usage" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commands!$B$1:$B$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commands!$B$1:$B$38</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
   <si>
     <t>VALIDATE SCRIPT scriptName</t>
   </si>
@@ -277,6 +278,9 @@
   </si>
   <si>
     <t>schedules/-/running-state</t>
+  </si>
+  <si>
+    <t>scripts/-/running/{scriptName}</t>
   </si>
 </sst>
 </file>
@@ -666,11 +670,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +735,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="4" t="str">
-        <f t="shared" ref="B4:B37" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
+        <f t="shared" ref="B4:B38" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
         <v>GET</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -787,30 +791,30 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>63</v>
+      <c r="A8" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="B8" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>--</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>GET</v>
+        <v>PUT</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>15</v>
@@ -818,14 +822,14 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v>GET</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>15</v>
@@ -833,74 +837,74 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="B11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>LIST</v>
+        <v>DELETE</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="4" t="str">
-        <f t="shared" ref="B12" si="2">LEFT(A12,SEARCH(" ",A12)-1)</f>
+      <c r="B13" s="4" t="str">
+        <f t="shared" ref="B13" si="2">LEFT(A13,SEARCH(" ",A13)-1)</f>
         <v>CREATE</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="4" t="str">
-        <f t="shared" ref="B13" si="3">LEFT(A13,SEARCH(" ",A13)-1)</f>
-        <v>UPDATE</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>73</v>
+      <c r="D13" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>71</v>
+      <c r="A14" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="B14" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
+        <f t="shared" ref="B14" si="3">LEFT(A14,SEARCH(" ",A14)-1)</f>
+        <v>UPDATE</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>18</v>
+      <c r="D14" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>SHOW</v>
+        <v>PUT</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>18</v>
@@ -908,119 +912,119 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>LIST</v>
+        <v>SHOW</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="4" t="str">
+      <c r="B18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>DELETE</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="4" t="str">
+      <c r="B19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>--</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>VALIDATE</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>VALIDATE</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="4" t="str">
+      <c r="B21" s="4" t="str">
         <f t="shared" si="1"/>
         <v>LIST</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="4" t="str">
-        <f t="shared" ref="B21" si="4">LEFT(A21,SEARCH(" ",A21)-1)</f>
+      <c r="B22" s="4" t="str">
+        <f t="shared" ref="B22" si="4">LEFT(A22,SEARCH(" ",A22)-1)</f>
         <v>--</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="C22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="4" t="str">
+      <c r="B23" s="4" t="str">
         <f t="shared" si="1"/>
         <v>CREATE</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>SHOW</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>19</v>
@@ -1028,52 +1032,52 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v>SHOW</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="4" t="str">
+      <c r="B26" s="4" t="str">
         <f t="shared" si="1"/>
         <v>UPDATE</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1083,49 +1087,49 @@
         <v>10</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="B28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>START</v>
+        <v>LIST</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B29" s="4" t="str">
-        <f>LEFT(A29,SEARCH(" ",A29)-1)</f>
-        <v>STOP</v>
+        <f t="shared" si="1"/>
+        <v>START</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B30" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>SHOW</v>
+        <f>LEFT(A30,SEARCH(" ",A30)-1)</f>
+        <v>STOP</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>33</v>
@@ -1133,44 +1137,44 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B31" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>LIST</v>
+        <v>SHOW</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>STOP</v>
+        <v>LIST</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B33" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>START</v>
+        <v>STOP</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>22</v>
@@ -1178,14 +1182,14 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>CONFIRM</v>
+        <v>START</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>22</v>
@@ -1193,46 +1197,61 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B35" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>STOP</v>
+        <v>CONFIRM</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B36" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>CREATE</v>
+        <v>STOP</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CREATE</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="4" t="str">
+      <c r="B38" s="4" t="str">
         <f t="shared" si="1"/>
         <v>CONFIRM</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="C38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make sourcefiles and targetfiles resources functional and document them
</commit_message>
<xml_diff>
--- a/docs/DBPA manager web service URIs.xlsx
+++ b/docs/DBPA manager web service URIs.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\hauldata\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593F0DCD-3063-4D9F-ABD8-C5F806C9CEAC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C0977F-D617-4607-A3BC-38542F8003A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
     <sheet name="Usage" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commands!$B$1:$B$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commands!$B$1:$B$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
   <si>
     <t>VALIDATE SCRIPT scriptName</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>VALIDATE SCHEDULE schedName</t>
-  </si>
-  <si>
-    <t>scripts/-/validations/{scriptName}</t>
   </si>
   <si>
     <t>schedules/-/validations/{schedName}</t>
@@ -281,6 +278,24 @@
   </si>
   <si>
     <t>scripts/-/running/{scriptName}</t>
+  </si>
+  <si>
+    <t>sourcefiles/{fileName}</t>
+  </si>
+  <si>
+    <t>scripts/{scriptName}/rename</t>
+  </si>
+  <si>
+    <t>scripts/{scriptName}/validation</t>
+  </si>
+  <si>
+    <t>scripts/validate</t>
+  </si>
+  <si>
+    <t>scripts/-/validations[?like={likeName}]</t>
+  </si>
+  <si>
+    <t>targetfiles/{fileName}</t>
   </si>
 </sst>
 </file>
@@ -670,11 +685,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +706,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>8</v>
@@ -702,7 +717,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="4" t="str">
         <f>LEFT(A2,SEARCH(" ",A2)-1)</f>
@@ -717,7 +732,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="4" t="str">
         <f t="shared" ref="B3" si="0">LEFT(A3,SEARCH(" ",A3)-1)</f>
@@ -732,10 +747,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="str">
-        <f t="shared" ref="B4:B38" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
+        <f t="shared" ref="B4:B45" si="1">LEFT(A4,SEARCH(" ",A4)-1)</f>
         <v>GET</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -746,203 +761,203 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
+      <c r="A5" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="B5" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v>--</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="B6" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>LIST</v>
+        <v>DELETE</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="str">
+      <c r="B8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>VALIDATE</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="4" t="str">
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>--</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>64</v>
+      <c r="A10" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="B10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>GET</v>
+        <v>--</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>2</v>
+      <c r="A11" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="B11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v>--</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="4" t="str">
+        <f t="shared" ref="B12:B15" si="2">LEFT(A12,SEARCH(" ",A12)-1)</f>
+        <v>--</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>--</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="4" t="str">
-        <f t="shared" ref="B13" si="2">LEFT(A13,SEARCH(" ",A13)-1)</f>
-        <v>CREATE</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>72</v>
+      <c r="A14" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="B14" s="4" t="str">
-        <f t="shared" ref="B14" si="3">LEFT(A14,SEARCH(" ",A14)-1)</f>
-        <v>UPDATE</v>
+        <f t="shared" si="2"/>
+        <v>--</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>73</v>
+        <v>10</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>71</v>
+      <c r="A15" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="B15" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
+        <f t="shared" si="2"/>
+        <v>--</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="B16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>SHOW</v>
+        <v>PUT</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>LIST</v>
+        <v>GET</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B18" s="4" t="str">
         <f t="shared" si="1"/>
@@ -952,102 +967,102 @@
         <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>60</v>
+      <c r="A19" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>--</v>
+        <v>LIST</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="B20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>VALIDATE</v>
+        <f t="shared" ref="B20" si="3">LEFT(A20,SEARCH(" ",A20)-1)</f>
+        <v>CREATE</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>46</v>
+      <c r="A21" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="B21" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>LIST</v>
+        <f t="shared" ref="B21" si="4">LEFT(A21,SEARCH(" ",A21)-1)</f>
+        <v>UPDATE</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>60</v>
+      <c r="A22" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B22" s="4" t="str">
-        <f t="shared" ref="B22" si="4">LEFT(A22,SEARCH(" ",A22)-1)</f>
-        <v>--</v>
+        <f t="shared" si="1"/>
+        <v>PUT</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>70</v>
+        <v>11</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>CREATE</v>
+        <v>SHOW</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>SHOW</v>
+        <v>LIST</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B25" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1057,42 +1072,42 @@
         <v>14</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>65</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="B26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>66</v>
+        <v>--</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>LIST</v>
+        <v>VALIDATE</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B28" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1102,42 +1117,42 @@
         <v>10</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>68</v>
+      <c r="A29" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="B29" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>START</v>
+        <f t="shared" ref="B29" si="5">LEFT(A29,SEARCH(" ",A29)-1)</f>
+        <v>--</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B30" s="4" t="str">
-        <f>LEFT(A30,SEARCH(" ",A30)-1)</f>
-        <v>STOP</v>
+        <f t="shared" si="1"/>
+        <v>CREATE</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="B31" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1147,111 +1162,216 @@
         <v>10</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="B32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>LIST</v>
+        <v>DELETE</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B33" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>STOP</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>22</v>
+        <v>UPDATE</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B34" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>START</v>
+        <v>LIST</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B35" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>CONFIRM</v>
+        <v>LIST</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B36" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>STOP</v>
+        <v>START</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B37" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>CREATE</v>
+        <f>LEFT(A37,SEARCH(" ",A37)-1)</f>
+        <v>STOP</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>SHOW</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>LIST</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>STOP</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>START</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CONFIRM</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>STOP</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CREATE</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="4" t="str">
+      <c r="B45" s="4" t="str">
         <f t="shared" si="1"/>
         <v>CONFIRM</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="C45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1277,10 +1397,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1288,7 +1408,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1296,23 +1416,23 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1320,7 +1440,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>